<commit_message>
Create Real-time-chat and update send email
</commit_message>
<xml_diff>
--- a/backend/src/main/resources/data/doctors/doctors.xlsx
+++ b/backend/src/main/resources/data/doctors/doctors.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="316">
   <si>
     <t>name</t>
   </si>
@@ -148,10 +148,13 @@
 </t>
   </si>
   <si>
-    <t>Chuyên gia ngoại khoa, phẫu thuật tiêu hoá</t>
-  </si>
-  <si>
-    <t>Việt Đức - Trung tâm Ngoại</t>
+    <t>BSCKII Phạm Hải Bằng</t>
+  </si>
+  <si>
+    <t>Chuyên gia phẫu thuật tổng hợp</t>
+  </si>
+  <si>
+    <t>BV Việt Đức - TT Cấp cứu và Điều trị ban ngày</t>
   </si>
   <si>
     <t>/images/doctors/6.png</t>
@@ -172,8 +175,7 @@
     <t>/images/doctors/7.png</t>
   </si>
   <si>
-    <t xml:space="preserve">PGS.TS Nguyễn Hữu Ước là bác sĩ có nhiều kinh nghiệm trong phẫu thuật tim mạch, tham gia điều trị các bệnh lý phức tạp về tim và mạch máu. Ông thường xuyên xử lý các trường hợp cấp cứu tim mạch, kết hợp với các chuyên khoa liên quan để mang lại phác đồ tối ưu cho bệnh nhân. Bác sĩ tích cực tham gia đào tạo và hướng dẫn kỹ thuật phẫu thuật tim cho bác sĩ nội trú và đồng nghiệp, đồng thời góp phần xây dựng quy trình chăm sóc sau mổ dành cho bệnh nhân tim. Với sự tận tâm và kinh nghiệm sâu sắc, bác sĩ được bệnh nhân tin tưởng trong những trường hợp khó về tim mạch.
-</t>
+    <t>BSCKII Phạm Hải Bằng là chuyên gia phẫu thuật với thế mạnh nổi bật trong xử trí các bệnh lý nhiễm trùng và tổn thương phức tạp vùng ngực, bụng và vùng đầu cổ. Bác sĩ có nhiều kinh nghiệm trong phẫu thuật điều trị sẹo hẹp khí quản, giúp phục hồi chức năng hô hấp cho những trường hợp khó. Bên cạnh đó, bác sĩ còn thành thạo phẫu thuật áp-xe sàn miệng – cổ – trung thất, cũng như các can thiệp mủ màng phổi, ổ cặn màng phổi và áp-xe phổi. Ở lĩnh vực tiêu hóa, bác sĩ thực hiện hiệu quả các phẫu thuật điều trị nhiễm khuẩn ổ bụng và rò tiêu hóa. Ngoài ra, BSCKII Phạm Hải Bằng còn có kinh nghiệm sâu trong phẫu thuật hậu môn – trực tràng và tầng sinh môn, mang lại kết quả điều trị an toàn và tối ưu cho người bệnh.</t>
   </si>
   <si>
     <t>GS.TS Trần Trung Dũng</t>
@@ -993,7 +995,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_-* #,##0\ &quot;₫&quot;_-;\-* #,##0\ &quot;₫&quot;_-;_-* &quot;-&quot;\ &quot;₫&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1003,13 +1005,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1479,148 +1474,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1986,8 +1981,8 @@
   <sheetPr/>
   <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -2158,19 +2153,19 @@
     </row>
     <row r="7" ht="103" customHeight="1" spans="1:8">
       <c r="A7" s="3" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F7" s="3">
         <v>2</v>
@@ -2184,19 +2179,19 @@
     </row>
     <row r="8" ht="89" customHeight="1" spans="1:8">
       <c r="A8" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F8" s="3">
         <v>2</v>
@@ -2205,24 +2200,24 @@
         <v>2</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" ht="99" customHeight="1" spans="1:8">
       <c r="A9" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F9" s="3">
         <v>2</v>
@@ -2231,24 +2226,24 @@
         <v>16</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" ht="113" customHeight="1" spans="1:8">
       <c r="A10" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F10" s="3">
         <v>2</v>
@@ -2257,24 +2252,24 @@
         <v>19</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" ht="103" customHeight="1" spans="1:8">
       <c r="A11" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F11" s="3">
         <v>2</v>
@@ -2283,24 +2278,24 @@
         <v>6</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F12" s="3">
         <v>3</v>
@@ -2312,19 +2307,19 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F13" s="3">
         <v>3</v>
@@ -2336,19 +2331,19 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F14" s="3">
         <v>3</v>
@@ -2360,19 +2355,19 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F15" s="3">
         <v>3</v>
@@ -2384,19 +2379,19 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F16" s="3">
         <v>3</v>
@@ -2408,19 +2403,19 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F17" s="3">
         <v>4</v>
@@ -2432,19 +2427,19 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F18" s="3">
         <v>4</v>
@@ -2456,19 +2451,19 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F19" s="3">
         <v>4</v>
@@ -2480,19 +2475,19 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F20" s="3">
         <v>4</v>
@@ -2504,19 +2499,19 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F21" s="3">
         <v>4</v>
@@ -2528,19 +2523,19 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F22" s="3">
         <v>5</v>
@@ -2552,19 +2547,19 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F23" s="3">
         <v>5</v>
@@ -2576,19 +2571,19 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F24" s="3">
         <v>5</v>
@@ -2600,19 +2595,19 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F25" s="3">
         <v>5</v>
@@ -2624,19 +2619,19 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F26" s="3">
         <v>5</v>
@@ -2648,19 +2643,19 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F27" s="3">
         <v>6</v>
@@ -2672,19 +2667,19 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F28" s="3">
         <v>6</v>
@@ -2696,19 +2691,19 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F29" s="3">
         <v>6</v>
@@ -2720,19 +2715,19 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F30" s="3">
         <v>6</v>
@@ -2744,19 +2739,19 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F31" s="3">
         <v>6</v>
@@ -2768,19 +2763,19 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F32" s="3">
         <v>7</v>
@@ -2792,19 +2787,19 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F33" s="3">
         <v>7</v>
@@ -2816,19 +2811,19 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F34" s="3">
         <v>7</v>
@@ -2840,19 +2835,19 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F35" s="3">
         <v>7</v>
@@ -2864,19 +2859,19 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F36" s="3">
         <v>7</v>
@@ -2888,19 +2883,19 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F37" s="3">
         <v>8</v>
@@ -2912,19 +2907,19 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F38" s="3">
         <v>8</v>
@@ -2936,19 +2931,19 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F39" s="3">
         <v>8</v>
@@ -2960,19 +2955,19 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F40" s="3">
         <v>8</v>
@@ -2984,19 +2979,19 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F41" s="3">
         <v>8</v>
@@ -3008,19 +3003,19 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F42" s="3">
         <v>9</v>
@@ -3032,19 +3027,19 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F43" s="3">
         <v>9</v>
@@ -3056,19 +3051,19 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F44" s="3">
         <v>9</v>
@@ -3080,19 +3075,19 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F45" s="3">
         <v>9</v>
@@ -3104,19 +3099,19 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F46" s="3">
         <v>9</v>
@@ -3128,19 +3123,19 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F47" s="3">
         <v>10</v>
@@ -3152,19 +3147,19 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F48" s="3">
         <v>10</v>
@@ -3176,19 +3171,19 @@
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F49" s="3">
         <v>10</v>
@@ -3200,7 +3195,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>27</v>
@@ -3209,10 +3204,10 @@
         <v>28</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F50" s="3">
         <v>10</v>
@@ -3224,19 +3219,19 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F51" s="3">
         <v>10</v>
@@ -3248,19 +3243,19 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F52" s="3">
         <v>11</v>
@@ -3272,19 +3267,19 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="F53" s="3">
         <v>11</v>
@@ -3296,19 +3291,19 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F54" s="3">
         <v>11</v>
@@ -3320,19 +3315,19 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F55" s="3">
         <v>11</v>
@@ -3344,19 +3339,19 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F56" s="3">
         <v>11</v>
@@ -3368,19 +3363,19 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F57" s="3">
         <v>12</v>
@@ -3392,19 +3387,19 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="3" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F58" s="3">
         <v>12</v>
@@ -3416,7 +3411,7 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>27</v>
@@ -3425,10 +3420,10 @@
         <v>28</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="F59" s="3">
         <v>12</v>
@@ -3440,19 +3435,19 @@
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="3" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F60" s="3">
         <v>12</v>
@@ -3464,19 +3459,19 @@
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="3" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F61" s="3">
         <v>12</v>
@@ -3488,19 +3483,19 @@
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F62" s="3">
         <v>13</v>
@@ -3512,19 +3507,19 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F63" s="3">
         <v>13</v>
@@ -3536,19 +3531,19 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" s="3" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F64" s="3">
         <v>13</v>
@@ -3560,19 +3555,19 @@
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="3" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="F65" s="3">
         <v>13</v>
@@ -3584,7 +3579,7 @@
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="3" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>27</v>
@@ -3593,10 +3588,10 @@
         <v>28</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F66" s="3">
         <v>13</v>
@@ -3608,19 +3603,19 @@
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="3" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="F67" s="3">
         <v>14</v>
@@ -3632,19 +3627,19 @@
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="3" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="F68" s="3">
         <v>14</v>
@@ -3656,19 +3651,19 @@
     </row>
     <row r="69" spans="1:8">
       <c r="A69" s="3" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="F69" s="3">
         <v>14</v>
@@ -3680,19 +3675,19 @@
     </row>
     <row r="70" spans="1:8">
       <c r="A70" s="3" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="F70" s="3">
         <v>14</v>
@@ -3704,19 +3699,19 @@
     </row>
     <row r="71" spans="1:8">
       <c r="A71" s="3" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="F71" s="3">
         <v>14</v>
@@ -3728,19 +3723,19 @@
     </row>
     <row r="72" spans="1:8">
       <c r="A72" s="3" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="F72" s="3">
         <v>15</v>
@@ -3752,19 +3747,19 @@
     </row>
     <row r="73" spans="1:8">
       <c r="A73" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F73" s="3">
         <v>15</v>
@@ -3776,19 +3771,19 @@
     </row>
     <row r="74" spans="1:8">
       <c r="A74" s="3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F74" s="3">
         <v>15</v>
@@ -3800,19 +3795,19 @@
     </row>
     <row r="75" spans="1:8">
       <c r="A75" s="3" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F75" s="3">
         <v>15</v>
@@ -3824,19 +3819,19 @@
     </row>
     <row r="76" spans="1:8">
       <c r="A76" s="3" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F76" s="3">
         <v>15</v>

</xml_diff>